<commit_message>
Adds CF for H
</commit_message>
<xml_diff>
--- a/premise_gwp/data/lcia_gwp_100a.xlsx
+++ b/premise_gwp/data/lcia_gwp_100a.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="59">
   <si>
     <t>name</t>
   </si>
@@ -35,12 +35,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>Carbon dioxide, in air</t>
-  </si>
-  <si>
-    <t>Carbon dioxide, non-fossil</t>
-  </si>
-  <si>
     <t>Carbon dioxide, fossil</t>
   </si>
   <si>
@@ -176,9 +170,6 @@
     <t>VOC, volatile organic compounds, unspecified origin</t>
   </si>
   <si>
-    <t>natural resource::in air</t>
-  </si>
-  <si>
     <t>air::lower stratosphere + upper troposphere</t>
   </si>
   <si>
@@ -209,7 +200,7 @@
     <t>soil::unspecified</t>
   </si>
   <si>
-    <t>Carbon dioxide, non-fossil, resource correction</t>
+    <t>Hydrogen</t>
   </si>
 </sst>
 </file>
@@ -570,19 +561,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C219"/>
+  <dimension ref="A1:C218"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="44.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,73 +584,73 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C2">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C3">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -670,51 +661,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -722,43 +713,43 @@
         <v>54</v>
       </c>
       <c r="C13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C14">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
         <v>56</v>
       </c>
-      <c r="C14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" t="s">
-        <v>55</v>
-      </c>
       <c r="C15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -766,2228 +757,2217 @@
         <v>52</v>
       </c>
       <c r="C17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.0624000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.0624000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.0624000000000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C20">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.0624000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C21">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.0624000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C22">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.0624000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C23">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4.0624000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C24">
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C25">
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C26">
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C27">
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C28">
-        <v>4.0624000000000002</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.4910000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C29">
-        <v>4.0624000000000002</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.4910000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C30">
-        <v>4.0624000000000002</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.4910000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31">
-        <v>4.0624000000000002</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.4910000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32">
-        <v>4.0624000000000002</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2.4910000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>9</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33">
-        <v>4.0624000000000002</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16.40180896</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>9</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C34">
-        <v>4.0624000000000002</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16.40180896</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C35">
-        <v>2.4910000000000001</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16.40180896</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C36">
-        <v>2.4910000000000001</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16.40180896</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C37">
-        <v>2.4910000000000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16.40180896</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C38">
-        <v>2.4910000000000001</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>264.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C39">
-        <v>2.4910000000000001</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>264.8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C40">
-        <v>16.40180896</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>264.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41">
-        <v>16.40180896</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>264.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C42">
-        <v>16.40180896</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>264.8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>11</v>
       </c>
       <c r="B43" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C43">
-        <v>16.40180896</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1301.2701999599999</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>11</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C44">
-        <v>16.40180896</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1301.2701999599999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C45">
-        <v>264.8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1301.2701999599999</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C46">
-        <v>264.8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1301.2701999599999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B47" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47">
-        <v>264.8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1301.2701999599999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>12</v>
       </c>
       <c r="B48" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C48">
-        <v>264.8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>160.09863099</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>12</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C49">
-        <v>264.8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>160.09863099</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B50" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C50">
-        <v>1301.2701999599999</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>160.09863099</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B51" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51">
-        <v>1301.2701999599999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>160.09863099</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52">
-        <v>1301.2701999599999</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>160.09863099</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>13</v>
       </c>
       <c r="B53" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C53">
-        <v>1301.2701999599999</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4804.43907777</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>13</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C54">
-        <v>1301.2701999599999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4804.43907777</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B55" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C55">
-        <v>160.09863099</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4804.43907777</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C56">
-        <v>160.09863099</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4804.43907777</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C57">
-        <v>160.09863099</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4804.43907777</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C58">
-        <v>160.09863099</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5823.7261870100001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>14</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C59">
-        <v>160.09863099</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5823.7261870100001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C60">
-        <v>4804.43907777</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5823.7261870100001</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B61" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C61">
-        <v>4804.43907777</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5823.7261870100001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B62" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C62">
-        <v>4804.43907777</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5823.7261870100001</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>15</v>
       </c>
       <c r="B63" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C63">
-        <v>4804.43907777</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>782.03725985999995</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>15</v>
       </c>
       <c r="B64" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C64">
-        <v>4804.43907777</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>782.03725985999995</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B65" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C65">
-        <v>5823.7261870100001</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>782.03725985999995</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B66" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C66">
-        <v>5823.7261870100001</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>782.03725985999995</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B67" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C67">
-        <v>5823.7261870100001</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>782.03725985999995</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>16</v>
       </c>
       <c r="B68" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C68">
-        <v>5823.7261870100001</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137.56020393</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>16</v>
       </c>
       <c r="B69" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C69">
-        <v>5823.7261870100001</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137.56020393</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B70" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C70">
-        <v>782.03725985999995</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137.56020393</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C71">
-        <v>782.03725985999995</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137.56020393</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B72" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C72">
-        <v>782.03725985999995</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>137.56020393</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>17</v>
       </c>
       <c r="B73" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C73">
-        <v>782.03725985999995</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.89826216999999997</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>17</v>
       </c>
       <c r="B74" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C74">
-        <v>782.03725985999995</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.89826216999999997</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B75" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C75">
-        <v>137.56020393</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.89826216999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B76" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C76">
-        <v>137.56020393</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.89826216999999997</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B77" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C77">
-        <v>137.56020393</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>0.89826216999999997</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>18</v>
       </c>
       <c r="B78" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C78">
-        <v>137.56020393</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8592.2020844899998</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>18</v>
       </c>
       <c r="B79" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C79">
-        <v>137.56020393</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8592.2020844899998</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B80" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C80">
-        <v>0.89826216999999997</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8592.2020844899998</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B81" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C81">
-        <v>0.89826216999999997</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8592.2020844899998</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B82" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C82">
-        <v>0.89826216999999997</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8592.2020844899998</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>19</v>
       </c>
       <c r="B83" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C83">
-        <v>0.89826216999999997</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1982.0354626599999</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>19</v>
       </c>
       <c r="B84" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C84">
-        <v>0.89826216999999997</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1982.0354626599999</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B85" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C85">
-        <v>8592.2020844899998</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1982.0354626599999</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B86" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C86">
-        <v>8592.2020844899998</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1982.0354626599999</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B87" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C87">
-        <v>8592.2020844899998</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1982.0354626599999</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>20</v>
       </c>
       <c r="B88" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C88">
-        <v>8592.2020844899998</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79.367176749999999</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>20</v>
       </c>
       <c r="B89" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C89">
-        <v>8592.2020844899998</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79.367176749999999</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B90" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C90">
-        <v>1982.0354626599999</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79.367176749999999</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B91" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C91">
-        <v>1982.0354626599999</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79.367176749999999</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B92" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C92">
-        <v>1982.0354626599999</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+        <v>79.367176749999999</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>21</v>
       </c>
       <c r="B93" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C93">
-        <v>1982.0354626599999</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>526.54777691000004</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>21</v>
       </c>
       <c r="B94" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C94">
-        <v>1982.0354626599999</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>526.54777691000004</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B95" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C95">
-        <v>79.367176749999999</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>526.54777691000004</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B96" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C96">
-        <v>79.367176749999999</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <v>526.54777691000004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B97" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C97">
-        <v>79.367176749999999</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>526.54777691000004</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>22</v>
       </c>
       <c r="B98" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C98">
-        <v>79.367176749999999</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7665.36131656</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>22</v>
       </c>
       <c r="B99" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C99">
-        <v>79.367176749999999</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7665.36131656</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B100" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C100">
-        <v>526.54777691000004</v>
-      </c>
-    </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7665.36131656</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B101" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C101">
-        <v>526.54777691000004</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7665.36131656</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B102" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C102">
-        <v>526.54777691000004</v>
-      </c>
-    </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7665.36131656</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>23</v>
       </c>
       <c r="B103" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C103">
-        <v>526.54777691000004</v>
-      </c>
-    </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11123.49391992</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>23</v>
       </c>
       <c r="B104" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C104">
-        <v>526.54777691000004</v>
-      </c>
-    </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11123.49391992</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B105" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C105">
-        <v>7665.36131656</v>
-      </c>
-    </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11123.49391992</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B106" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C106">
-        <v>7665.36131656</v>
-      </c>
-    </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11123.49391992</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B107" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C107">
-        <v>7665.36131656</v>
-      </c>
-    </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11123.49391992</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>24</v>
       </c>
       <c r="B108" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C108">
-        <v>7665.36131656</v>
-      </c>
-    </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3169.2551762200001</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>24</v>
       </c>
       <c r="B109" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C109">
-        <v>7665.36131656</v>
-      </c>
-    </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3169.2551762200001</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
+        <v>24</v>
+      </c>
+      <c r="B110" t="s">
+        <v>49</v>
+      </c>
+      <c r="C110">
+        <v>3169.2551762200001</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>24</v>
+      </c>
+      <c r="B111" t="s">
+        <v>50</v>
+      </c>
+      <c r="C111">
+        <v>3169.2551762200001</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>24</v>
+      </c>
+      <c r="B112" t="s">
+        <v>51</v>
+      </c>
+      <c r="C112">
+        <v>3169.2551762200001</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>58</v>
+      </c>
+      <c r="B113" t="s">
+        <v>52</v>
+      </c>
+      <c r="C113">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>58</v>
+      </c>
+      <c r="B114" t="s">
+        <v>48</v>
+      </c>
+      <c r="C114">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>58</v>
+      </c>
+      <c r="B115" t="s">
+        <v>49</v>
+      </c>
+      <c r="C115">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A116" t="s">
+        <v>58</v>
+      </c>
+      <c r="B116" t="s">
+        <v>50</v>
+      </c>
+      <c r="C116">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A117" t="s">
+        <v>58</v>
+      </c>
+      <c r="B117" t="s">
+        <v>51</v>
+      </c>
+      <c r="C117">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A118" t="s">
         <v>25</v>
       </c>
-      <c r="B110" t="s">
-        <v>55</v>
-      </c>
-      <c r="C110">
-        <v>11123.49391992</v>
-      </c>
-    </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="B118" t="s">
+        <v>51</v>
+      </c>
+      <c r="C118">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A119" t="s">
         <v>25</v>
       </c>
-      <c r="B111" t="s">
-        <v>51</v>
-      </c>
-      <c r="C111">
-        <v>11123.49391992</v>
-      </c>
-    </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>25</v>
-      </c>
-      <c r="B112" t="s">
-        <v>52</v>
-      </c>
-      <c r="C112">
-        <v>11123.49391992</v>
-      </c>
-    </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>25</v>
-      </c>
-      <c r="B113" t="s">
-        <v>53</v>
-      </c>
-      <c r="C113">
-        <v>11123.49391992</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
-        <v>25</v>
-      </c>
-      <c r="B114" t="s">
-        <v>54</v>
-      </c>
-      <c r="C114">
-        <v>11123.49391992</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="B119" t="s">
+        <v>51</v>
+      </c>
+      <c r="C119">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A120" t="s">
         <v>26</v>
       </c>
-      <c r="B115" t="s">
-        <v>55</v>
-      </c>
-      <c r="C115">
-        <v>3169.2551762200001</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="B120" t="s">
+        <v>52</v>
+      </c>
+      <c r="C120">
+        <v>2.3545465000000001</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A121" t="s">
         <v>26</v>
       </c>
-      <c r="B116" t="s">
-        <v>51</v>
-      </c>
-      <c r="C116">
-        <v>3169.2551762200001</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>26</v>
-      </c>
-      <c r="B117" t="s">
-        <v>52</v>
-      </c>
-      <c r="C117">
-        <v>3169.2551762200001</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>26</v>
-      </c>
-      <c r="B118" t="s">
-        <v>53</v>
-      </c>
-      <c r="C118">
-        <v>3169.2551762200001</v>
-      </c>
-    </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>26</v>
-      </c>
-      <c r="B119" t="s">
-        <v>54</v>
-      </c>
-      <c r="C119">
-        <v>3169.2551762200001</v>
-      </c>
-    </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>27</v>
-      </c>
-      <c r="B120" t="s">
-        <v>54</v>
-      </c>
-      <c r="C120">
-        <v>29.7</v>
-      </c>
-    </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>28</v>
-      </c>
       <c r="B121" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C121">
         <v>2.3545465000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B122" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C122">
         <v>2.3545465000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B123" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C123">
         <v>2.3545465000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B124" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C124">
         <v>2.3545465000000001</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B125" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C125">
-        <v>2.3545465000000001</v>
-      </c>
-    </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1746.48198701</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B126" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C126">
         <v>1746.48198701</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B127" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C127">
         <v>1746.48198701</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B128" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C128">
         <v>1746.48198701</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B129" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C129">
         <v>1746.48198701</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B130" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C130">
-        <v>1746.48198701</v>
-      </c>
-    </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6291.6295759499999</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B131" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C131">
         <v>6291.6295759499999</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B132" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C132">
         <v>6291.6295759499999</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B133" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C133">
         <v>6291.6295759499999</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B134" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C134">
         <v>6291.6295759499999</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B135" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C135">
-        <v>6291.6295759499999</v>
-      </c>
-    </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1764.6295088100001</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B136" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C136">
         <v>1764.6295088100001</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B137" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C137">
         <v>1764.6295088100001</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B138" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C138">
         <v>1764.6295088100001</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B139" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C139">
         <v>1764.6295088100001</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B140" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C140">
-        <v>1764.6295088100001</v>
-      </c>
-    </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13893.35260104</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B141" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C141">
         <v>13893.35260104</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B142" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C142">
         <v>13893.35260104</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B143" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C143">
         <v>13893.35260104</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B144" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C144">
         <v>13893.35260104</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B145" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C145">
-        <v>13893.35260104</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8.9151945999999995</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B146" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C146">
         <v>8.9151945999999995</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B147" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C147">
         <v>8.9151945999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B148" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C148">
         <v>8.9151945999999995</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B149" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C149">
         <v>8.9151945999999995</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B150" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C150">
-        <v>8.9151945999999995</v>
-      </c>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10239.234599179999</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B151" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C151">
         <v>10239.234599179999</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B152" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C152">
         <v>10239.234599179999</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B153" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C153">
         <v>10239.234599179999</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B154" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C154">
         <v>10239.234599179999</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B155" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C155">
-        <v>10239.234599179999</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+        <v>147.66224518000001</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B156" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C156">
         <v>147.66224518000001</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B157" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C157">
         <v>147.66224518000001</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B158" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C158">
         <v>147.66224518000001</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B159" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C159">
         <v>147.66224518000001</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B160" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C160">
-        <v>147.66224518000001</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+        <v>676.80778461</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B161" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C161">
         <v>676.80778461</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B162" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C162">
         <v>676.80778461</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B163" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C163">
         <v>676.80778461</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B164" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C164">
         <v>676.80778461</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B165" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C165">
-        <v>676.80778461</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B166" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C166">
         <v>29.7</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B167" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C167">
         <v>29.7</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B168" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C168">
         <v>29.7</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B169" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C169">
         <v>29.7</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B170" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C170">
         <v>29.7</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B171" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C171">
         <v>29.7</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B172" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C172">
         <v>29.7</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B173" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C173">
         <v>29.7</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B174" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C174">
         <v>29.7</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B175" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C175">
         <v>29.7</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B176" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C176">
-        <v>29.7</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12.18322764</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B177" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C177">
         <v>12.18322764</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B178" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C178">
         <v>12.18322764</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B179" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C179">
         <v>12.18322764</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B180" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C180">
         <v>12.18322764</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B181" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C181">
-        <v>12.18322764</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B182" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C182">
         <v>28.5</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B183" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C183">
         <v>28.5</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B184" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C184">
         <v>28.5</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B185" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C185">
         <v>28.5</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B186" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C186">
-        <v>28.5</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1728.47068126</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B187" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C187">
         <v>1728.47068126</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B188" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C188">
         <v>1728.47068126</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B189" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C189">
         <v>1728.47068126</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B190" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C190">
         <v>1728.47068126</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B191" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C191">
-        <v>1728.47068126</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6625.7804207700001</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B192" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C192">
         <v>6625.7804207700001</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B193" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C193">
         <v>6625.7804207700001</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B194" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C194">
         <v>6625.7804207700001</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B195" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C195">
         <v>6625.7804207700001</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B196" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C196">
-        <v>6625.7804207700001</v>
-      </c>
-    </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4662.9369943800002</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B197" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C197">
         <v>4662.9369943800002</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B198" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C198">
         <v>4662.9369943800002</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B199" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C199">
         <v>4662.9369943800002</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B200" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C200">
         <v>4662.9369943800002</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B201" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C201">
-        <v>4662.9369943800002</v>
-      </c>
-    </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12397.60343847</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B202" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C202">
         <v>12397.60343847</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B203" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C203">
         <v>12397.60343847</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B204" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C204">
         <v>12397.60343847</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B205" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C205">
         <v>12397.60343847</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
+        <v>43</v>
+      </c>
+      <c r="B206" t="s">
+        <v>50</v>
+      </c>
+      <c r="C206">
+        <v>-10.8</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A207" t="s">
         <v>44</v>
       </c>
-      <c r="B206" t="s">
-        <v>54</v>
-      </c>
-      <c r="C206">
-        <v>12397.60343847</v>
-      </c>
-    </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>45</v>
-      </c>
       <c r="B207" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C207">
-        <v>-10.8</v>
-      </c>
-    </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16069.99763401</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B208" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C208">
         <v>16069.99763401</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B209" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C209">
         <v>16069.99763401</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B210" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C210">
         <v>16069.99763401</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B211" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C211">
         <v>16069.99763401</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
+        <v>45</v>
+      </c>
+      <c r="B212" t="s">
+        <v>50</v>
+      </c>
+      <c r="C212">
+        <v>8546.7045304599997</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A213" t="s">
         <v>46</v>
       </c>
-      <c r="B212" t="s">
-        <v>54</v>
-      </c>
-      <c r="C212">
-        <v>16069.99763401</v>
-      </c>
-    </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>47</v>
-      </c>
       <c r="B213" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C213">
-        <v>8546.7045304599997</v>
-      </c>
-    </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+        <v>23506.819993159999</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B214" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C214">
         <v>23506.819993159999</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B215" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C215">
         <v>23506.819993159999</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B216" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C216">
         <v>23506.819993159999</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B217" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C217">
         <v>23506.819993159999</v>
       </c>
     </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B218" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C218">
-        <v>23506.819993159999</v>
-      </c>
-    </row>
-    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>49</v>
-      </c>
-      <c r="B219" t="s">
-        <v>53</v>
-      </c>
-      <c r="C219">
         <v>4.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update CF for H
</commit_message>
<xml_diff>
--- a/premise_gwp/data/lcia_gwp_100a.xlsx
+++ b/premise_gwp/data/lcia_gwp_100a.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="59">
   <si>
     <t>name</t>
   </si>
@@ -561,10 +561,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C218"/>
+  <dimension ref="A1:C217"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C124" sqref="C124"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1813,7 +1813,7 @@
         <v>52</v>
       </c>
       <c r="C113">
-        <v>4.3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
@@ -1824,7 +1824,7 @@
         <v>48</v>
       </c>
       <c r="C114">
-        <v>4.3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
@@ -1835,7 +1835,7 @@
         <v>49</v>
       </c>
       <c r="C115">
-        <v>4.3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
@@ -1846,7 +1846,7 @@
         <v>50</v>
       </c>
       <c r="C116">
-        <v>4.3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
@@ -1857,7 +1857,7 @@
         <v>51</v>
       </c>
       <c r="C117">
-        <v>4.3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
@@ -1868,18 +1868,18 @@
         <v>51</v>
       </c>
       <c r="C118">
-        <v>4.3</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B119" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C119">
-        <v>29.7</v>
+        <v>2.3545465000000001</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
@@ -1887,7 +1887,7 @@
         <v>26</v>
       </c>
       <c r="B120" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C120">
         <v>2.3545465000000001</v>
@@ -1898,7 +1898,7 @@
         <v>26</v>
       </c>
       <c r="B121" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C121">
         <v>2.3545465000000001</v>
@@ -1909,7 +1909,7 @@
         <v>26</v>
       </c>
       <c r="B122" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C122">
         <v>2.3545465000000001</v>
@@ -1920,7 +1920,7 @@
         <v>26</v>
       </c>
       <c r="B123" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C123">
         <v>2.3545465000000001</v>
@@ -1928,13 +1928,13 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B124" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C124">
-        <v>2.3545465000000001</v>
+        <v>1746.48198701</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
@@ -1942,7 +1942,7 @@
         <v>27</v>
       </c>
       <c r="B125" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C125">
         <v>1746.48198701</v>
@@ -1953,7 +1953,7 @@
         <v>27</v>
       </c>
       <c r="B126" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C126">
         <v>1746.48198701</v>
@@ -1964,7 +1964,7 @@
         <v>27</v>
       </c>
       <c r="B127" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C127">
         <v>1746.48198701</v>
@@ -1975,7 +1975,7 @@
         <v>27</v>
       </c>
       <c r="B128" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C128">
         <v>1746.48198701</v>
@@ -1983,13 +1983,13 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B129" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C129">
-        <v>1746.48198701</v>
+        <v>6291.6295759499999</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
@@ -1997,7 +1997,7 @@
         <v>28</v>
       </c>
       <c r="B130" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C130">
         <v>6291.6295759499999</v>
@@ -2008,7 +2008,7 @@
         <v>28</v>
       </c>
       <c r="B131" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C131">
         <v>6291.6295759499999</v>
@@ -2019,7 +2019,7 @@
         <v>28</v>
       </c>
       <c r="B132" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C132">
         <v>6291.6295759499999</v>
@@ -2030,7 +2030,7 @@
         <v>28</v>
       </c>
       <c r="B133" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C133">
         <v>6291.6295759499999</v>
@@ -2038,13 +2038,13 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B134" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C134">
-        <v>6291.6295759499999</v>
+        <v>1764.6295088100001</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
@@ -2052,7 +2052,7 @@
         <v>29</v>
       </c>
       <c r="B135" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C135">
         <v>1764.6295088100001</v>
@@ -2063,7 +2063,7 @@
         <v>29</v>
       </c>
       <c r="B136" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C136">
         <v>1764.6295088100001</v>
@@ -2074,7 +2074,7 @@
         <v>29</v>
       </c>
       <c r="B137" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C137">
         <v>1764.6295088100001</v>
@@ -2085,7 +2085,7 @@
         <v>29</v>
       </c>
       <c r="B138" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C138">
         <v>1764.6295088100001</v>
@@ -2093,13 +2093,13 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B139" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C139">
-        <v>1764.6295088100001</v>
+        <v>13893.35260104</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
@@ -2107,7 +2107,7 @@
         <v>30</v>
       </c>
       <c r="B140" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C140">
         <v>13893.35260104</v>
@@ -2118,7 +2118,7 @@
         <v>30</v>
       </c>
       <c r="B141" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C141">
         <v>13893.35260104</v>
@@ -2129,7 +2129,7 @@
         <v>30</v>
       </c>
       <c r="B142" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C142">
         <v>13893.35260104</v>
@@ -2140,7 +2140,7 @@
         <v>30</v>
       </c>
       <c r="B143" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C143">
         <v>13893.35260104</v>
@@ -2148,13 +2148,13 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B144" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C144">
-        <v>13893.35260104</v>
+        <v>8.9151945999999995</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
@@ -2162,7 +2162,7 @@
         <v>31</v>
       </c>
       <c r="B145" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C145">
         <v>8.9151945999999995</v>
@@ -2173,7 +2173,7 @@
         <v>31</v>
       </c>
       <c r="B146" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C146">
         <v>8.9151945999999995</v>
@@ -2184,7 +2184,7 @@
         <v>31</v>
       </c>
       <c r="B147" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C147">
         <v>8.9151945999999995</v>
@@ -2195,7 +2195,7 @@
         <v>31</v>
       </c>
       <c r="B148" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C148">
         <v>8.9151945999999995</v>
@@ -2203,13 +2203,13 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B149" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C149">
-        <v>8.9151945999999995</v>
+        <v>10239.234599179999</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
@@ -2217,7 +2217,7 @@
         <v>32</v>
       </c>
       <c r="B150" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C150">
         <v>10239.234599179999</v>
@@ -2228,7 +2228,7 @@
         <v>32</v>
       </c>
       <c r="B151" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C151">
         <v>10239.234599179999</v>
@@ -2239,7 +2239,7 @@
         <v>32</v>
       </c>
       <c r="B152" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C152">
         <v>10239.234599179999</v>
@@ -2250,7 +2250,7 @@
         <v>32</v>
       </c>
       <c r="B153" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C153">
         <v>10239.234599179999</v>
@@ -2258,13 +2258,13 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B154" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C154">
-        <v>10239.234599179999</v>
+        <v>147.66224518000001</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
@@ -2272,7 +2272,7 @@
         <v>33</v>
       </c>
       <c r="B155" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C155">
         <v>147.66224518000001</v>
@@ -2283,7 +2283,7 @@
         <v>33</v>
       </c>
       <c r="B156" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C156">
         <v>147.66224518000001</v>
@@ -2294,7 +2294,7 @@
         <v>33</v>
       </c>
       <c r="B157" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C157">
         <v>147.66224518000001</v>
@@ -2305,7 +2305,7 @@
         <v>33</v>
       </c>
       <c r="B158" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C158">
         <v>147.66224518000001</v>
@@ -2313,13 +2313,13 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B159" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C159">
-        <v>147.66224518000001</v>
+        <v>676.80778461</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
@@ -2327,7 +2327,7 @@
         <v>34</v>
       </c>
       <c r="B160" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C160">
         <v>676.80778461</v>
@@ -2338,7 +2338,7 @@
         <v>34</v>
       </c>
       <c r="B161" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C161">
         <v>676.80778461</v>
@@ -2349,7 +2349,7 @@
         <v>34</v>
       </c>
       <c r="B162" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C162">
         <v>676.80778461</v>
@@ -2360,7 +2360,7 @@
         <v>34</v>
       </c>
       <c r="B163" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C163">
         <v>676.80778461</v>
@@ -2368,13 +2368,13 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B164" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C164">
-        <v>676.80778461</v>
+        <v>29.7</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
@@ -2382,7 +2382,7 @@
         <v>35</v>
       </c>
       <c r="B165" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C165">
         <v>29.7</v>
@@ -2393,7 +2393,7 @@
         <v>35</v>
       </c>
       <c r="B166" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C166">
         <v>29.7</v>
@@ -2404,7 +2404,7 @@
         <v>35</v>
       </c>
       <c r="B167" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C167">
         <v>29.7</v>
@@ -2415,7 +2415,7 @@
         <v>35</v>
       </c>
       <c r="B168" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C168">
         <v>29.7</v>
@@ -2423,10 +2423,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B169" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C169">
         <v>29.7</v>
@@ -2437,7 +2437,7 @@
         <v>36</v>
       </c>
       <c r="B170" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C170">
         <v>29.7</v>
@@ -2448,7 +2448,7 @@
         <v>36</v>
       </c>
       <c r="B171" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C171">
         <v>29.7</v>
@@ -2459,7 +2459,7 @@
         <v>36</v>
       </c>
       <c r="B172" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C172">
         <v>29.7</v>
@@ -2470,7 +2470,7 @@
         <v>36</v>
       </c>
       <c r="B173" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C173">
         <v>29.7</v>
@@ -2481,7 +2481,7 @@
         <v>36</v>
       </c>
       <c r="B174" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C174">
         <v>29.7</v>
@@ -2489,13 +2489,13 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B175" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C175">
-        <v>29.7</v>
+        <v>12.18322764</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
@@ -2503,7 +2503,7 @@
         <v>37</v>
       </c>
       <c r="B176" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C176">
         <v>12.18322764</v>
@@ -2514,7 +2514,7 @@
         <v>37</v>
       </c>
       <c r="B177" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C177">
         <v>12.18322764</v>
@@ -2525,7 +2525,7 @@
         <v>37</v>
       </c>
       <c r="B178" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C178">
         <v>12.18322764</v>
@@ -2536,7 +2536,7 @@
         <v>37</v>
       </c>
       <c r="B179" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C179">
         <v>12.18322764</v>
@@ -2544,13 +2544,13 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B180" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C180">
-        <v>12.18322764</v>
+        <v>28.5</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
@@ -2558,7 +2558,7 @@
         <v>38</v>
       </c>
       <c r="B181" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C181">
         <v>28.5</v>
@@ -2569,7 +2569,7 @@
         <v>38</v>
       </c>
       <c r="B182" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C182">
         <v>28.5</v>
@@ -2580,7 +2580,7 @@
         <v>38</v>
       </c>
       <c r="B183" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C183">
         <v>28.5</v>
@@ -2591,7 +2591,7 @@
         <v>38</v>
       </c>
       <c r="B184" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C184">
         <v>28.5</v>
@@ -2599,13 +2599,13 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B185" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C185">
-        <v>28.5</v>
+        <v>1728.47068126</v>
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
@@ -2613,7 +2613,7 @@
         <v>39</v>
       </c>
       <c r="B186" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C186">
         <v>1728.47068126</v>
@@ -2624,7 +2624,7 @@
         <v>39</v>
       </c>
       <c r="B187" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C187">
         <v>1728.47068126</v>
@@ -2635,7 +2635,7 @@
         <v>39</v>
       </c>
       <c r="B188" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C188">
         <v>1728.47068126</v>
@@ -2646,7 +2646,7 @@
         <v>39</v>
       </c>
       <c r="B189" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C189">
         <v>1728.47068126</v>
@@ -2654,13 +2654,13 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B190" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C190">
-        <v>1728.47068126</v>
+        <v>6625.7804207700001</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
@@ -2668,7 +2668,7 @@
         <v>40</v>
       </c>
       <c r="B191" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C191">
         <v>6625.7804207700001</v>
@@ -2679,7 +2679,7 @@
         <v>40</v>
       </c>
       <c r="B192" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C192">
         <v>6625.7804207700001</v>
@@ -2690,7 +2690,7 @@
         <v>40</v>
       </c>
       <c r="B193" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C193">
         <v>6625.7804207700001</v>
@@ -2701,7 +2701,7 @@
         <v>40</v>
       </c>
       <c r="B194" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C194">
         <v>6625.7804207700001</v>
@@ -2709,13 +2709,13 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B195" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C195">
-        <v>6625.7804207700001</v>
+        <v>4662.9369943800002</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
@@ -2723,7 +2723,7 @@
         <v>41</v>
       </c>
       <c r="B196" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C196">
         <v>4662.9369943800002</v>
@@ -2734,7 +2734,7 @@
         <v>41</v>
       </c>
       <c r="B197" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C197">
         <v>4662.9369943800002</v>
@@ -2745,7 +2745,7 @@
         <v>41</v>
       </c>
       <c r="B198" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C198">
         <v>4662.9369943800002</v>
@@ -2756,7 +2756,7 @@
         <v>41</v>
       </c>
       <c r="B199" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C199">
         <v>4662.9369943800002</v>
@@ -2764,13 +2764,13 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B200" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C200">
-        <v>4662.9369943800002</v>
+        <v>12397.60343847</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
@@ -2778,7 +2778,7 @@
         <v>42</v>
       </c>
       <c r="B201" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C201">
         <v>12397.60343847</v>
@@ -2789,7 +2789,7 @@
         <v>42</v>
       </c>
       <c r="B202" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C202">
         <v>12397.60343847</v>
@@ -2800,7 +2800,7 @@
         <v>42</v>
       </c>
       <c r="B203" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C203">
         <v>12397.60343847</v>
@@ -2811,7 +2811,7 @@
         <v>42</v>
       </c>
       <c r="B204" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C204">
         <v>12397.60343847</v>
@@ -2819,24 +2819,24 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B205" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C205">
-        <v>12397.60343847</v>
+        <v>-10.8</v>
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B206" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C206">
-        <v>-10.8</v>
+        <v>16069.99763401</v>
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
@@ -2844,7 +2844,7 @@
         <v>44</v>
       </c>
       <c r="B207" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C207">
         <v>16069.99763401</v>
@@ -2855,7 +2855,7 @@
         <v>44</v>
       </c>
       <c r="B208" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C208">
         <v>16069.99763401</v>
@@ -2866,7 +2866,7 @@
         <v>44</v>
       </c>
       <c r="B209" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C209">
         <v>16069.99763401</v>
@@ -2877,7 +2877,7 @@
         <v>44</v>
       </c>
       <c r="B210" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C210">
         <v>16069.99763401</v>
@@ -2885,24 +2885,24 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B211" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C211">
-        <v>16069.99763401</v>
+        <v>8546.7045304599997</v>
       </c>
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B212" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C212">
-        <v>8546.7045304599997</v>
+        <v>23506.819993159999</v>
       </c>
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.3">
@@ -2910,7 +2910,7 @@
         <v>46</v>
       </c>
       <c r="B213" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C213">
         <v>23506.819993159999</v>
@@ -2921,7 +2921,7 @@
         <v>46</v>
       </c>
       <c r="B214" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C214">
         <v>23506.819993159999</v>
@@ -2932,7 +2932,7 @@
         <v>46</v>
       </c>
       <c r="B215" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C215">
         <v>23506.819993159999</v>
@@ -2943,7 +2943,7 @@
         <v>46</v>
       </c>
       <c r="B216" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C216">
         <v>23506.819993159999</v>
@@ -2951,23 +2951,12 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B217" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C217">
-        <v>23506.819993159999</v>
-      </c>
-    </row>
-    <row r="218" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A218" t="s">
-        <v>47</v>
-      </c>
-      <c r="B218" t="s">
-        <v>50</v>
-      </c>
-      <c r="C218">
         <v>4.5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update CF for hydrogen to 11 kg CO2-eq./kg.
</commit_message>
<xml_diff>
--- a/premise_gwp/data/lcia_gwp_100a.xlsx
+++ b/premise_gwp/data/lcia_gwp_100a.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10313"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sacchi_r\Documents\GitHub\premise_gwp\premise_gwp\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/premise_gwp/premise_gwp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8541314-1AF5-5746-AB56-181E8CEEE2C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13500"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="28800" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913" calcMode="manual" iterate="1" iterateCount="5"/>
+  <calcPr calcId="162913" calcMode="manual" iterate="1" iterateCount="10" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -206,7 +207,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -560,20 +561,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C217"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="C124" sqref="C124"/>
+      <selection activeCell="B112" sqref="B112"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="44.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,7 +585,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -595,7 +596,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -606,7 +607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -617,7 +618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -628,7 +629,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -639,7 +640,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -650,7 +651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -661,7 +662,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -672,7 +673,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
@@ -683,7 +684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
@@ -694,7 +695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>4</v>
       </c>
@@ -705,7 +706,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>5</v>
       </c>
@@ -716,7 +717,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>5</v>
       </c>
@@ -727,7 +728,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>5</v>
       </c>
@@ -738,7 +739,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>5</v>
       </c>
@@ -749,7 +750,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>6</v>
       </c>
@@ -760,7 +761,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -771,7 +772,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>6</v>
       </c>
@@ -782,7 +783,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -793,7 +794,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>6</v>
       </c>
@@ -804,7 +805,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>7</v>
       </c>
@@ -815,7 +816,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>7</v>
       </c>
@@ -826,7 +827,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>7</v>
       </c>
@@ -837,7 +838,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>7</v>
       </c>
@@ -848,7 +849,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>7</v>
       </c>
@@ -859,7 +860,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -870,7 +871,7 @@
         <v>4.0624000000000002</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -881,7 +882,7 @@
         <v>2.4910000000000001</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>8</v>
       </c>
@@ -892,7 +893,7 @@
         <v>2.4910000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -903,7 +904,7 @@
         <v>2.4910000000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>8</v>
       </c>
@@ -914,7 +915,7 @@
         <v>2.4910000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -925,7 +926,7 @@
         <v>2.4910000000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -936,7 +937,7 @@
         <v>16.40180896</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -947,7 +948,7 @@
         <v>16.40180896</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -958,7 +959,7 @@
         <v>16.40180896</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -969,7 +970,7 @@
         <v>16.40180896</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -980,7 +981,7 @@
         <v>16.40180896</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -991,7 +992,7 @@
         <v>264.8</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1002,7 +1003,7 @@
         <v>264.8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1013,7 +1014,7 @@
         <v>264.8</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>10</v>
       </c>
@@ -1024,7 +1025,7 @@
         <v>264.8</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>264.8</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>11</v>
       </c>
@@ -1046,7 +1047,7 @@
         <v>1301.2701999599999</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>11</v>
       </c>
@@ -1057,7 +1058,7 @@
         <v>1301.2701999599999</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>11</v>
       </c>
@@ -1068,7 +1069,7 @@
         <v>1301.2701999599999</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -1079,7 +1080,7 @@
         <v>1301.2701999599999</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1090,7 +1091,7 @@
         <v>1301.2701999599999</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>12</v>
       </c>
@@ -1101,7 +1102,7 @@
         <v>160.09863099</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>12</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>160.09863099</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>12</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>160.09863099</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>12</v>
       </c>
@@ -1134,7 +1135,7 @@
         <v>160.09863099</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>12</v>
       </c>
@@ -1145,7 +1146,7 @@
         <v>160.09863099</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>13</v>
       </c>
@@ -1156,7 +1157,7 @@
         <v>4804.43907777</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>13</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>4804.43907777</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>13</v>
       </c>
@@ -1178,7 +1179,7 @@
         <v>4804.43907777</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>13</v>
       </c>
@@ -1189,7 +1190,7 @@
         <v>4804.43907777</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>13</v>
       </c>
@@ -1200,7 +1201,7 @@
         <v>4804.43907777</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>14</v>
       </c>
@@ -1211,7 +1212,7 @@
         <v>5823.7261870100001</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>14</v>
       </c>
@@ -1222,7 +1223,7 @@
         <v>5823.7261870100001</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>14</v>
       </c>
@@ -1233,7 +1234,7 @@
         <v>5823.7261870100001</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>14</v>
       </c>
@@ -1244,7 +1245,7 @@
         <v>5823.7261870100001</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>14</v>
       </c>
@@ -1255,7 +1256,7 @@
         <v>5823.7261870100001</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>15</v>
       </c>
@@ -1266,7 +1267,7 @@
         <v>782.03725985999995</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>15</v>
       </c>
@@ -1277,7 +1278,7 @@
         <v>782.03725985999995</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>15</v>
       </c>
@@ -1288,7 +1289,7 @@
         <v>782.03725985999995</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>15</v>
       </c>
@@ -1299,7 +1300,7 @@
         <v>782.03725985999995</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>15</v>
       </c>
@@ -1310,7 +1311,7 @@
         <v>782.03725985999995</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>16</v>
       </c>
@@ -1321,7 +1322,7 @@
         <v>137.56020393</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>16</v>
       </c>
@@ -1332,7 +1333,7 @@
         <v>137.56020393</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>16</v>
       </c>
@@ -1343,7 +1344,7 @@
         <v>137.56020393</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>16</v>
       </c>
@@ -1354,7 +1355,7 @@
         <v>137.56020393</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>16</v>
       </c>
@@ -1365,7 +1366,7 @@
         <v>137.56020393</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>17</v>
       </c>
@@ -1376,7 +1377,7 @@
         <v>0.89826216999999997</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>17</v>
       </c>
@@ -1387,7 +1388,7 @@
         <v>0.89826216999999997</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>17</v>
       </c>
@@ -1398,7 +1399,7 @@
         <v>0.89826216999999997</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>17</v>
       </c>
@@ -1409,7 +1410,7 @@
         <v>0.89826216999999997</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>17</v>
       </c>
@@ -1420,7 +1421,7 @@
         <v>0.89826216999999997</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>18</v>
       </c>
@@ -1431,7 +1432,7 @@
         <v>8592.2020844899998</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>18</v>
       </c>
@@ -1442,7 +1443,7 @@
         <v>8592.2020844899998</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>18</v>
       </c>
@@ -1453,7 +1454,7 @@
         <v>8592.2020844899998</v>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>18</v>
       </c>
@@ -1464,7 +1465,7 @@
         <v>8592.2020844899998</v>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>18</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>8592.2020844899998</v>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>19</v>
       </c>
@@ -1486,7 +1487,7 @@
         <v>1982.0354626599999</v>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>19</v>
       </c>
@@ -1497,7 +1498,7 @@
         <v>1982.0354626599999</v>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>19</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>1982.0354626599999</v>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>19</v>
       </c>
@@ -1519,7 +1520,7 @@
         <v>1982.0354626599999</v>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>19</v>
       </c>
@@ -1530,7 +1531,7 @@
         <v>1982.0354626599999</v>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>20</v>
       </c>
@@ -1541,7 +1542,7 @@
         <v>79.367176749999999</v>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>20</v>
       </c>
@@ -1552,7 +1553,7 @@
         <v>79.367176749999999</v>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>20</v>
       </c>
@@ -1563,7 +1564,7 @@
         <v>79.367176749999999</v>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>20</v>
       </c>
@@ -1574,7 +1575,7 @@
         <v>79.367176749999999</v>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>20</v>
       </c>
@@ -1585,7 +1586,7 @@
         <v>79.367176749999999</v>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>21</v>
       </c>
@@ -1596,7 +1597,7 @@
         <v>526.54777691000004</v>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>21</v>
       </c>
@@ -1607,7 +1608,7 @@
         <v>526.54777691000004</v>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>21</v>
       </c>
@@ -1618,7 +1619,7 @@
         <v>526.54777691000004</v>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>21</v>
       </c>
@@ -1629,7 +1630,7 @@
         <v>526.54777691000004</v>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>21</v>
       </c>
@@ -1640,7 +1641,7 @@
         <v>526.54777691000004</v>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>22</v>
       </c>
@@ -1651,7 +1652,7 @@
         <v>7665.36131656</v>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>22</v>
       </c>
@@ -1662,7 +1663,7 @@
         <v>7665.36131656</v>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>22</v>
       </c>
@@ -1673,7 +1674,7 @@
         <v>7665.36131656</v>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>22</v>
       </c>
@@ -1684,7 +1685,7 @@
         <v>7665.36131656</v>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>22</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>7665.36131656</v>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>23</v>
       </c>
@@ -1706,7 +1707,7 @@
         <v>11123.49391992</v>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>23</v>
       </c>
@@ -1717,7 +1718,7 @@
         <v>11123.49391992</v>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>23</v>
       </c>
@@ -1728,7 +1729,7 @@
         <v>11123.49391992</v>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>23</v>
       </c>
@@ -1739,7 +1740,7 @@
         <v>11123.49391992</v>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>23</v>
       </c>
@@ -1750,7 +1751,7 @@
         <v>11123.49391992</v>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>24</v>
       </c>
@@ -1761,7 +1762,7 @@
         <v>3169.2551762200001</v>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>24</v>
       </c>
@@ -1772,7 +1773,7 @@
         <v>3169.2551762200001</v>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>24</v>
       </c>
@@ -1783,7 +1784,7 @@
         <v>3169.2551762200001</v>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>24</v>
       </c>
@@ -1794,7 +1795,7 @@
         <v>3169.2551762200001</v>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>24</v>
       </c>
@@ -1805,7 +1806,7 @@
         <v>3169.2551762200001</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>58</v>
       </c>
@@ -1813,10 +1814,10 @@
         <v>52</v>
       </c>
       <c r="C113">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>58</v>
       </c>
@@ -1824,10 +1825,10 @@
         <v>48</v>
       </c>
       <c r="C114">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>58</v>
       </c>
@@ -1835,10 +1836,10 @@
         <v>49</v>
       </c>
       <c r="C115">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>58</v>
       </c>
@@ -1846,10 +1847,10 @@
         <v>50</v>
       </c>
       <c r="C116">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>58</v>
       </c>
@@ -1857,10 +1858,10 @@
         <v>51</v>
       </c>
       <c r="C117">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>25</v>
       </c>
@@ -1871,7 +1872,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>26</v>
       </c>
@@ -1882,7 +1883,7 @@
         <v>2.3545465000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>26</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>2.3545465000000001</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>26</v>
       </c>
@@ -1904,7 +1905,7 @@
         <v>2.3545465000000001</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>26</v>
       </c>
@@ -1915,7 +1916,7 @@
         <v>2.3545465000000001</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>26</v>
       </c>
@@ -1926,7 +1927,7 @@
         <v>2.3545465000000001</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>27</v>
       </c>
@@ -1937,7 +1938,7 @@
         <v>1746.48198701</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>27</v>
       </c>
@@ -1948,7 +1949,7 @@
         <v>1746.48198701</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>27</v>
       </c>
@@ -1959,7 +1960,7 @@
         <v>1746.48198701</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>27</v>
       </c>
@@ -1970,7 +1971,7 @@
         <v>1746.48198701</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>27</v>
       </c>
@@ -1981,7 +1982,7 @@
         <v>1746.48198701</v>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>28</v>
       </c>
@@ -1992,7 +1993,7 @@
         <v>6291.6295759499999</v>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>28</v>
       </c>
@@ -2003,7 +2004,7 @@
         <v>6291.6295759499999</v>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>28</v>
       </c>
@@ -2014,7 +2015,7 @@
         <v>6291.6295759499999</v>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>28</v>
       </c>
@@ -2025,7 +2026,7 @@
         <v>6291.6295759499999</v>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>28</v>
       </c>
@@ -2036,7 +2037,7 @@
         <v>6291.6295759499999</v>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>29</v>
       </c>
@@ -2047,7 +2048,7 @@
         <v>1764.6295088100001</v>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>29</v>
       </c>
@@ -2058,7 +2059,7 @@
         <v>1764.6295088100001</v>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>29</v>
       </c>
@@ -2069,7 +2070,7 @@
         <v>1764.6295088100001</v>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>29</v>
       </c>
@@ -2080,7 +2081,7 @@
         <v>1764.6295088100001</v>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>29</v>
       </c>
@@ -2091,7 +2092,7 @@
         <v>1764.6295088100001</v>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>30</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>13893.35260104</v>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>30</v>
       </c>
@@ -2113,7 +2114,7 @@
         <v>13893.35260104</v>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>30</v>
       </c>
@@ -2124,7 +2125,7 @@
         <v>13893.35260104</v>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>30</v>
       </c>
@@ -2135,7 +2136,7 @@
         <v>13893.35260104</v>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>30</v>
       </c>
@@ -2146,7 +2147,7 @@
         <v>13893.35260104</v>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>31</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>8.9151945999999995</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>31</v>
       </c>
@@ -2168,7 +2169,7 @@
         <v>8.9151945999999995</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>31</v>
       </c>
@@ -2179,7 +2180,7 @@
         <v>8.9151945999999995</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>31</v>
       </c>
@@ -2190,7 +2191,7 @@
         <v>8.9151945999999995</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>31</v>
       </c>
@@ -2201,7 +2202,7 @@
         <v>8.9151945999999995</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>32</v>
       </c>
@@ -2212,7 +2213,7 @@
         <v>10239.234599179999</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>32</v>
       </c>
@@ -2223,7 +2224,7 @@
         <v>10239.234599179999</v>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>32</v>
       </c>
@@ -2234,7 +2235,7 @@
         <v>10239.234599179999</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>32</v>
       </c>
@@ -2245,7 +2246,7 @@
         <v>10239.234599179999</v>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>32</v>
       </c>
@@ -2256,7 +2257,7 @@
         <v>10239.234599179999</v>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>33</v>
       </c>
@@ -2267,7 +2268,7 @@
         <v>147.66224518000001</v>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>33</v>
       </c>
@@ -2278,7 +2279,7 @@
         <v>147.66224518000001</v>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>33</v>
       </c>
@@ -2289,7 +2290,7 @@
         <v>147.66224518000001</v>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>33</v>
       </c>
@@ -2300,7 +2301,7 @@
         <v>147.66224518000001</v>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>33</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>147.66224518000001</v>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>34</v>
       </c>
@@ -2322,7 +2323,7 @@
         <v>676.80778461</v>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>34</v>
       </c>
@@ -2333,7 +2334,7 @@
         <v>676.80778461</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>34</v>
       </c>
@@ -2344,7 +2345,7 @@
         <v>676.80778461</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>34</v>
       </c>
@@ -2355,7 +2356,7 @@
         <v>676.80778461</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>34</v>
       </c>
@@ -2366,7 +2367,7 @@
         <v>676.80778461</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>35</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>35</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>35</v>
       </c>
@@ -2399,7 +2400,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>35</v>
       </c>
@@ -2410,7 +2411,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>35</v>
       </c>
@@ -2421,7 +2422,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>36</v>
       </c>
@@ -2432,7 +2433,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>36</v>
       </c>
@@ -2443,7 +2444,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>36</v>
       </c>
@@ -2454,7 +2455,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>36</v>
       </c>
@@ -2465,7 +2466,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>36</v>
       </c>
@@ -2476,7 +2477,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>36</v>
       </c>
@@ -2487,7 +2488,7 @@
         <v>29.7</v>
       </c>
     </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>37</v>
       </c>
@@ -2498,7 +2499,7 @@
         <v>12.18322764</v>
       </c>
     </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>37</v>
       </c>
@@ -2509,7 +2510,7 @@
         <v>12.18322764</v>
       </c>
     </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>37</v>
       </c>
@@ -2520,7 +2521,7 @@
         <v>12.18322764</v>
       </c>
     </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>37</v>
       </c>
@@ -2531,7 +2532,7 @@
         <v>12.18322764</v>
       </c>
     </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>37</v>
       </c>
@@ -2542,7 +2543,7 @@
         <v>12.18322764</v>
       </c>
     </row>
-    <row r="180" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>38</v>
       </c>
@@ -2553,7 +2554,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="181" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>38</v>
       </c>
@@ -2564,7 +2565,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="182" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>38</v>
       </c>
@@ -2575,7 +2576,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="183" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>38</v>
       </c>
@@ -2586,7 +2587,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="184" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>38</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="185" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>39</v>
       </c>
@@ -2608,7 +2609,7 @@
         <v>1728.47068126</v>
       </c>
     </row>
-    <row r="186" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>39</v>
       </c>
@@ -2619,7 +2620,7 @@
         <v>1728.47068126</v>
       </c>
     </row>
-    <row r="187" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>39</v>
       </c>
@@ -2630,7 +2631,7 @@
         <v>1728.47068126</v>
       </c>
     </row>
-    <row r="188" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>39</v>
       </c>
@@ -2641,7 +2642,7 @@
         <v>1728.47068126</v>
       </c>
     </row>
-    <row r="189" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>39</v>
       </c>
@@ -2652,7 +2653,7 @@
         <v>1728.47068126</v>
       </c>
     </row>
-    <row r="190" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>40</v>
       </c>
@@ -2663,7 +2664,7 @@
         <v>6625.7804207700001</v>
       </c>
     </row>
-    <row r="191" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>40</v>
       </c>
@@ -2674,7 +2675,7 @@
         <v>6625.7804207700001</v>
       </c>
     </row>
-    <row r="192" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>40</v>
       </c>
@@ -2685,7 +2686,7 @@
         <v>6625.7804207700001</v>
       </c>
     </row>
-    <row r="193" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>40</v>
       </c>
@@ -2696,7 +2697,7 @@
         <v>6625.7804207700001</v>
       </c>
     </row>
-    <row r="194" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>40</v>
       </c>
@@ -2707,7 +2708,7 @@
         <v>6625.7804207700001</v>
       </c>
     </row>
-    <row r="195" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>41</v>
       </c>
@@ -2718,7 +2719,7 @@
         <v>4662.9369943800002</v>
       </c>
     </row>
-    <row r="196" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>41</v>
       </c>
@@ -2729,7 +2730,7 @@
         <v>4662.9369943800002</v>
       </c>
     </row>
-    <row r="197" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>41</v>
       </c>
@@ -2740,7 +2741,7 @@
         <v>4662.9369943800002</v>
       </c>
     </row>
-    <row r="198" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>41</v>
       </c>
@@ -2751,7 +2752,7 @@
         <v>4662.9369943800002</v>
       </c>
     </row>
-    <row r="199" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>41</v>
       </c>
@@ -2762,7 +2763,7 @@
         <v>4662.9369943800002</v>
       </c>
     </row>
-    <row r="200" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>42</v>
       </c>
@@ -2773,7 +2774,7 @@
         <v>12397.60343847</v>
       </c>
     </row>
-    <row r="201" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>42</v>
       </c>
@@ -2784,7 +2785,7 @@
         <v>12397.60343847</v>
       </c>
     </row>
-    <row r="202" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>42</v>
       </c>
@@ -2795,7 +2796,7 @@
         <v>12397.60343847</v>
       </c>
     </row>
-    <row r="203" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>42</v>
       </c>
@@ -2806,7 +2807,7 @@
         <v>12397.60343847</v>
       </c>
     </row>
-    <row r="204" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>42</v>
       </c>
@@ -2817,7 +2818,7 @@
         <v>12397.60343847</v>
       </c>
     </row>
-    <row r="205" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>43</v>
       </c>
@@ -2828,7 +2829,7 @@
         <v>-10.8</v>
       </c>
     </row>
-    <row r="206" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>44</v>
       </c>
@@ -2839,7 +2840,7 @@
         <v>16069.99763401</v>
       </c>
     </row>
-    <row r="207" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>44</v>
       </c>
@@ -2850,7 +2851,7 @@
         <v>16069.99763401</v>
       </c>
     </row>
-    <row r="208" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>44</v>
       </c>
@@ -2861,7 +2862,7 @@
         <v>16069.99763401</v>
       </c>
     </row>
-    <row r="209" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>44</v>
       </c>
@@ -2872,7 +2873,7 @@
         <v>16069.99763401</v>
       </c>
     </row>
-    <row r="210" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>44</v>
       </c>
@@ -2883,7 +2884,7 @@
         <v>16069.99763401</v>
       </c>
     </row>
-    <row r="211" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>45</v>
       </c>
@@ -2894,7 +2895,7 @@
         <v>8546.7045304599997</v>
       </c>
     </row>
-    <row r="212" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>46</v>
       </c>
@@ -2905,7 +2906,7 @@
         <v>23506.819993159999</v>
       </c>
     </row>
-    <row r="213" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>46</v>
       </c>
@@ -2916,7 +2917,7 @@
         <v>23506.819993159999</v>
       </c>
     </row>
-    <row r="214" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>46</v>
       </c>
@@ -2927,7 +2928,7 @@
         <v>23506.819993159999</v>
       </c>
     </row>
-    <row r="215" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>46</v>
       </c>
@@ -2938,7 +2939,7 @@
         <v>23506.819993159999</v>
       </c>
     </row>
-    <row r="216" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>46</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>23506.819993159999</v>
       </c>
     </row>
-    <row r="217" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>47</v>
       </c>

</xml_diff>